<commit_message>
test d'un truc pour pouvoir modifier directement sur le site (avec l'aide du chat)
</commit_message>
<xml_diff>
--- a/data/livres.xlsx
+++ b/data/livres.xlsx
@@ -6043,9 +6043,9 @@
   <dimension ref="A1:G913"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A887" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A756" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="F917" activeCellId="0" sqref="F917"/>
+      <selection pane="bottomLeft" activeCell="F768" activeCellId="0" sqref="F768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>